<commit_message>
Tabla y gramatica corregida
</commit_message>
<xml_diff>
--- a/mimij/mimij/AnalisiSintactico/Tabla.xlsx
+++ b/mimij/mimij/AnalisiSintactico/Tabla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derly\Documents\Universidad\Sexto ciclo\Compis\Proyecto\Proyecto-Compiladores\mimij\mimij\bin\Debug\AnalisiSintactico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derly\Documents\Universidad\Sexto ciclo\Compis\Proyecto\Proyecto-Compiladores\mimij\mimij\AnalisiSintactico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB227ED-18CC-4A91-B1B0-7FE4BF45739F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AE6D8A-1316-4BD7-855F-9CE10AE83862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="15840" xr2:uid="{924D8882-C0E7-4292-B0BC-53CB839BE7C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{924D8882-C0E7-4292-B0BC-53CB839BE7C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="272">
   <si>
     <t>State</t>
   </si>
@@ -600,24 +600,12 @@
     <t>r54</t>
   </si>
   <si>
-    <t>s119</t>
-  </si>
-  <si>
     <t>r56</t>
   </si>
   <si>
-    <t>s120</t>
-  </si>
-  <si>
     <t>r58</t>
   </si>
   <si>
-    <t>s121</t>
-  </si>
-  <si>
-    <t>s122</t>
-  </si>
-  <si>
     <t>r61</t>
   </si>
   <si>
@@ -627,12 +615,6 @@
     <t>r63</t>
   </si>
   <si>
-    <t>s124</t>
-  </si>
-  <si>
-    <t>s125</t>
-  </si>
-  <si>
     <t>r66</t>
   </si>
   <si>
@@ -642,9 +624,6 @@
     <t>r69</t>
   </si>
   <si>
-    <t>s129</t>
-  </si>
-  <si>
     <t>r72</t>
   </si>
   <si>
@@ -823,6 +802,54 @@
   </si>
   <si>
     <t>r44</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>s119 / r54</t>
+  </si>
+  <si>
+    <t>s120 / r56</t>
+  </si>
+  <si>
+    <t>s121 / r58</t>
+  </si>
+  <si>
+    <t>s122 / r58</t>
+  </si>
+  <si>
+    <t>s124 / r63</t>
+  </si>
+  <si>
+    <t>s125 / r63</t>
+  </si>
+  <si>
+    <t>s129 / r69</t>
+  </si>
+  <si>
+    <t>s129 / r67</t>
+  </si>
+  <si>
+    <t>s129 / r68</t>
+  </si>
+  <si>
+    <t>s119 / r53</t>
+  </si>
+  <si>
+    <t>s120 / r55</t>
+  </si>
+  <si>
+    <t>s121 / r57</t>
+  </si>
+  <si>
+    <t>s122 / r57</t>
+  </si>
+  <si>
+    <t>s124 / r62</t>
+  </si>
+  <si>
+    <t>s125 / r62</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1207,7 @@
   <dimension ref="A1:BV176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="Q179" sqref="Q179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,8 +1437,8 @@
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>74</v>
@@ -9154,20 +9181,32 @@
       <c r="Z88" s="1"/>
       <c r="AA88" s="1"/>
       <c r="AB88" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AC88" s="1"/>
-      <c r="AD88" s="1"/>
-      <c r="AE88" s="1"/>
+        <v>257</v>
+      </c>
+      <c r="AC88" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD88" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE88" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="AF88" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AG88" s="1"/>
-      <c r="AH88" s="1"/>
+      <c r="AG88" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH88" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="AI88" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AJ88" s="1"/>
+      <c r="AJ88" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="AK88" s="1" t="s">
         <v>187</v>
       </c>
@@ -9226,16 +9265,16 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -9249,7 +9288,7 @@
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
@@ -9262,42 +9301,52 @@
       <c r="Z89" s="1"/>
       <c r="AA89" s="1"/>
       <c r="AB89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC89" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD89" s="1"/>
-      <c r="AE89" s="1"/>
+        <v>258</v>
+      </c>
+      <c r="AD89" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AE89" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AF89" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AG89" s="1"/>
-      <c r="AH89" s="1"/>
+        <v>188</v>
+      </c>
+      <c r="AG89" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH89" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AI89" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ89" s="1"/>
+        <v>188</v>
+      </c>
+      <c r="AJ89" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AK89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AL89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AM89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AN89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AO89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AP89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AQ89" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AR89" s="1"/>
       <c r="AS89" s="1"/>
@@ -9336,16 +9385,16 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -9359,7 +9408,7 @@
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
@@ -9372,46 +9421,52 @@
       <c r="Z90" s="1"/>
       <c r="AA90" s="1"/>
       <c r="AB90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AC90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD90" s="1" t="s">
-        <v>192</v>
+        <v>259</v>
       </c>
       <c r="AE90" s="1" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
       <c r="AF90" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AG90" s="1"/>
-      <c r="AH90" s="1"/>
+        <v>189</v>
+      </c>
+      <c r="AG90" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH90" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="AI90" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ90" s="1"/>
+        <v>189</v>
+      </c>
+      <c r="AJ90" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="AK90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AL90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AM90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AN90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AO90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AP90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AQ90" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AR90" s="1"/>
       <c r="AS90" s="1"/>
@@ -9450,16 +9505,16 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -9473,7 +9528,7 @@
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
       <c r="Q91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
@@ -9486,46 +9541,52 @@
       <c r="Z91" s="1"/>
       <c r="AA91" s="1"/>
       <c r="AB91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AC91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AD91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AE91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AF91" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG91" s="1"/>
-      <c r="AH91" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="AG91" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH91" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AI91" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AJ91" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="AJ91" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AK91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AL91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AM91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AN91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AO91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AP91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AQ91" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AR91" s="1"/>
       <c r="AS91" s="1"/>
@@ -9564,16 +9625,16 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -9587,7 +9648,7 @@
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
       <c r="Q92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
@@ -9600,50 +9661,52 @@
       <c r="Z92" s="1"/>
       <c r="AA92" s="1"/>
       <c r="AB92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AC92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AD92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AE92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AF92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AG92" s="1" t="s">
-        <v>197</v>
+        <v>261</v>
       </c>
       <c r="AH92" s="1" t="s">
-        <v>198</v>
+        <v>262</v>
       </c>
       <c r="AI92" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AJ92" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="AJ92" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="AK92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AL92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AM92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AN92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AO92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AP92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AQ92" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AR92" s="1"/>
       <c r="AS92" s="1"/>
@@ -9682,16 +9745,16 @@
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -9705,7 +9768,7 @@
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
       <c r="Q93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
@@ -9718,50 +9781,52 @@
       <c r="Z93" s="1"/>
       <c r="AA93" s="1"/>
       <c r="AB93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AC93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AD93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AE93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AF93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AG93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AH93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AI93" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ93" s="1"/>
+        <v>193</v>
+      </c>
+      <c r="AJ93" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="AK93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AL93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AM93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AN93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AO93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AP93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AQ93" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AR93" s="1"/>
       <c r="AS93" s="1"/>
@@ -9800,7 +9865,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
@@ -9900,7 +9965,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
@@ -10000,16 +10065,16 @@
         <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -10023,7 +10088,7 @@
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
       <c r="Q96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
@@ -10036,52 +10101,52 @@
       <c r="Z96" s="1"/>
       <c r="AA96" s="1"/>
       <c r="AB96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AC96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AD96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AE96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AF96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AG96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AH96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AI96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AJ96" s="1" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="AK96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AL96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AM96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AN96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AO96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AP96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AQ96" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AR96" s="1"/>
       <c r="AS96" s="1"/>
@@ -10120,16 +10185,16 @@
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
@@ -10143,7 +10208,7 @@
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
       <c r="Q97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
@@ -10156,52 +10221,52 @@
       <c r="Z97" s="1"/>
       <c r="AA97" s="1"/>
       <c r="AB97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AC97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AD97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AE97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AF97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AG97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AH97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AI97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AJ97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AK97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AL97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AM97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AN97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AO97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AP97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AQ97" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="AR97" s="1"/>
       <c r="AS97" s="1"/>
@@ -10358,16 +10423,16 @@
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
@@ -10381,7 +10446,7 @@
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
       <c r="Q99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
@@ -10394,52 +10459,52 @@
       <c r="Z99" s="1"/>
       <c r="AA99" s="1"/>
       <c r="AB99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AC99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AD99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AE99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AF99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AG99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AH99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AI99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AJ99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AK99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AL99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AM99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AN99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AO99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AP99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AQ99" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AR99" s="1"/>
       <c r="AS99" s="1"/>
@@ -10480,7 +10545,7 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -10558,16 +10623,16 @@
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
@@ -10581,7 +10646,7 @@
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
       <c r="Q101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
@@ -10594,52 +10659,52 @@
       <c r="Z101" s="1"/>
       <c r="AA101" s="1"/>
       <c r="AB101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AC101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AD101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AE101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AF101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AG101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AH101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AI101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AJ101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AK101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AL101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AM101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AN101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AO101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AP101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AQ101" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AR101" s="1"/>
       <c r="AS101" s="1"/>
@@ -10678,16 +10743,16 @@
         <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
@@ -10701,7 +10766,7 @@
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
       <c r="Q102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
@@ -10714,52 +10779,52 @@
       <c r="Z102" s="1"/>
       <c r="AA102" s="1"/>
       <c r="AB102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AC102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AD102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AE102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AF102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AG102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AH102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AI102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AJ102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AK102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AL102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AM102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AN102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AO102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AP102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AQ102" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AR102" s="1"/>
       <c r="AS102" s="1"/>
@@ -10798,16 +10863,16 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -10821,7 +10886,7 @@
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
       <c r="Q103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
@@ -10834,52 +10899,52 @@
       <c r="Z103" s="1"/>
       <c r="AA103" s="1"/>
       <c r="AB103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AC103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AD103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AE103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AF103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AG103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AH103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AI103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AJ103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AK103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AL103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AM103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AN103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AO103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AP103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AQ103" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AR103" s="1"/>
       <c r="AS103" s="1"/>
@@ -10918,16 +10983,16 @@
         <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
@@ -10941,7 +11006,7 @@
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
       <c r="Q104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
@@ -10954,52 +11019,52 @@
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
       <c r="AB104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AC104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AD104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AE104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AF104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AG104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AH104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AI104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AJ104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AK104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AL104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AM104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AN104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AO104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AP104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AQ104" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="AR104" s="1"/>
       <c r="AS104" s="1"/>
@@ -11038,16 +11103,16 @@
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
@@ -11061,7 +11126,7 @@
       <c r="O105" s="1"/>
       <c r="P105" s="1"/>
       <c r="Q105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
@@ -11074,52 +11139,52 @@
       <c r="Z105" s="1"/>
       <c r="AA105" s="1"/>
       <c r="AB105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AC105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AD105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AE105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AF105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AG105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AH105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AI105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AJ105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AK105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AL105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AM105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AN105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AO105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AP105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AQ105" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="AR105" s="1"/>
       <c r="AS105" s="1"/>
@@ -11158,7 +11223,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -11385,7 +11450,7 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -11462,35 +11527,35 @@
         <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
       <c r="I109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="J109" s="1"/>
       <c r="K109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="O109" s="1"/>
       <c r="P109" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
@@ -11556,7 +11621,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -11565,24 +11630,24 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
       <c r="I110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="O110" s="1"/>
       <c r="P110" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
@@ -11648,69 +11713,69 @@
         <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O111" s="1"/>
       <c r="P111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
       <c r="T111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="U111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="V111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="W111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="X111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="Y111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="Z111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
@@ -11718,37 +11783,37 @@
       <c r="AD111" s="1"/>
       <c r="AE111" s="1"/>
       <c r="AF111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AG111" s="1"/>
       <c r="AH111" s="1"/>
       <c r="AI111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AL111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AM111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AN111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AO111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AP111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AQ111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AR111" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AS111" s="1"/>
       <c r="AT111" s="1"/>
@@ -11793,7 +11858,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
       <c r="I112" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -11866,22 +11931,22 @@
         <v>111</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -11894,25 +11959,25 @@
       <c r="R113" s="1"/>
       <c r="S113" s="1"/>
       <c r="T113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="V113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="W113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="X113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="Y113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="Z113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
@@ -11920,34 +11985,34 @@
       <c r="AD113" s="1"/>
       <c r="AE113" s="1"/>
       <c r="AF113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AG113" s="1"/>
       <c r="AH113" s="1"/>
       <c r="AI113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AL113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AM113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AN113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AO113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AP113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AQ113" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="AR113" s="1"/>
       <c r="AS113" s="1"/>
@@ -12340,22 +12405,22 @@
         <v>115</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -12368,25 +12433,25 @@
       <c r="R117" s="1"/>
       <c r="S117" s="1"/>
       <c r="T117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="V117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="W117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="X117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="Y117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="Z117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
@@ -12394,34 +12459,34 @@
       <c r="AD117" s="1"/>
       <c r="AE117" s="1"/>
       <c r="AF117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AG117" s="1"/>
       <c r="AH117" s="1"/>
       <c r="AI117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AL117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AM117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AN117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AO117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AP117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AQ117" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AR117" s="1"/>
       <c r="AS117" s="1"/>
@@ -12461,7 +12526,7 @@
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -12660,7 +12725,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
@@ -12776,7 +12841,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
@@ -12890,7 +12955,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
@@ -13002,7 +13067,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
@@ -13112,7 +13177,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
@@ -13222,7 +13287,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
@@ -13330,7 +13395,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1" t="s">
@@ -13436,7 +13501,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1" t="s">
@@ -13542,16 +13607,16 @@
         <v>126</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -13565,7 +13630,7 @@
       <c r="O128" s="1"/>
       <c r="P128" s="1"/>
       <c r="Q128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
@@ -13578,52 +13643,52 @@
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
       <c r="AB128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AC128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AD128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AE128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AF128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AG128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AH128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AI128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AJ128" s="1" t="s">
-        <v>202</v>
+        <v>264</v>
       </c>
       <c r="AK128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AL128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AM128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AN128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AO128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AP128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AQ128" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AR128" s="1"/>
       <c r="AS128" s="1"/>
@@ -13782,16 +13847,16 @@
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -13805,7 +13870,7 @@
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
       <c r="Q130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
@@ -13818,52 +13883,52 @@
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
       <c r="AB130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AC130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AD130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AE130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AF130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AG130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AH130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AI130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AJ130" s="1" t="s">
-        <v>202</v>
+        <v>265</v>
       </c>
       <c r="AK130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AL130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AM130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AN130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AO130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AP130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AQ130" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AR130" s="1"/>
       <c r="AS130" s="1"/>
@@ -13902,7 +13967,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -13985,7 +14050,7 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -14062,7 +14127,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -14143,7 +14208,7 @@
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -14222,69 +14287,69 @@
         <v>133</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="M135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="O135" s="1"/>
       <c r="P135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
       <c r="T135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="V135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="W135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Y135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="Z135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
@@ -14292,37 +14357,37 @@
       <c r="AD135" s="1"/>
       <c r="AE135" s="1"/>
       <c r="AF135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AG135" s="1"/>
       <c r="AH135" s="1"/>
       <c r="AI135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AJ135" s="1"/>
       <c r="AK135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AL135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AM135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AN135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AO135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AP135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AQ135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AR135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AS135" s="1"/>
       <c r="AT135" s="1"/>
@@ -14445,7 +14510,7 @@
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
@@ -14525,7 +14590,7 @@
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -14603,7 +14668,7 @@
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -14682,22 +14747,22 @@
         <v>138</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
@@ -14710,25 +14775,25 @@
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
       <c r="T140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="U140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="W140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="X140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="Y140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="Z140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
@@ -14736,34 +14801,34 @@
       <c r="AD140" s="1"/>
       <c r="AE140" s="1"/>
       <c r="AF140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AG140" s="1"/>
       <c r="AH140" s="1"/>
       <c r="AI140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AJ140" s="1"/>
       <c r="AK140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AL140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AM140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AN140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AO140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AP140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AQ140" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AR140" s="1"/>
       <c r="AS140" s="1"/>
@@ -14817,7 +14882,7 @@
       <c r="O141" s="1"/>
       <c r="P141" s="1"/>
       <c r="Q141" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
@@ -14901,7 +14966,7 @@
       <c r="O142" s="1"/>
       <c r="P142" s="1"/>
       <c r="Q142" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
@@ -15004,16 +15069,16 @@
         <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -15027,7 +15092,7 @@
       <c r="O143" s="1"/>
       <c r="P143" s="1"/>
       <c r="Q143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="R143" s="1"/>
       <c r="S143" s="1"/>
@@ -15040,40 +15105,52 @@
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
       <c r="AB143" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AC143" s="1"/>
-      <c r="AD143" s="1"/>
-      <c r="AE143" s="1"/>
+        <v>266</v>
+      </c>
+      <c r="AC143" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD143" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE143" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="AF143" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="AG143" s="1"/>
-      <c r="AH143" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="AG143" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH143" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="AI143" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ143" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="AJ143" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="AK143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AL143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AM143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AN143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AO143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AP143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AQ143" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AR143" s="1"/>
       <c r="AS143" s="1"/>
@@ -15112,16 +15189,16 @@
         <v>142</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
@@ -15135,7 +15212,7 @@
       <c r="O144" s="1"/>
       <c r="P144" s="1"/>
       <c r="Q144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="R144" s="1"/>
       <c r="S144" s="1"/>
@@ -15148,42 +15225,52 @@
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
       <c r="AB144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AC144" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD144" s="1"/>
-      <c r="AE144" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="AD144" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE144" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="AF144" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="AG144" s="1"/>
-      <c r="AH144" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="AG144" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH144" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="AI144" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="AJ144" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="AJ144" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="AK144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AL144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AM144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AN144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AO144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AP144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AQ144" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="AR144" s="1"/>
       <c r="AS144" s="1"/>
@@ -15222,16 +15309,16 @@
         <v>143</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
@@ -15245,7 +15332,7 @@
       <c r="O145" s="1"/>
       <c r="P145" s="1"/>
       <c r="Q145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
@@ -15258,46 +15345,52 @@
       <c r="Z145" s="1"/>
       <c r="AA145" s="1"/>
       <c r="AB145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AC145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AD145" s="1" t="s">
-        <v>192</v>
+        <v>268</v>
       </c>
       <c r="AE145" s="1" t="s">
-        <v>193</v>
+        <v>269</v>
       </c>
       <c r="AF145" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AG145" s="1"/>
-      <c r="AH145" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="AG145" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH145" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="AI145" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AJ145" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="AJ145" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="AK145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AL145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AM145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AN145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AO145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AP145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AQ145" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="AR145" s="1"/>
       <c r="AS145" s="1"/>
@@ -15336,16 +15429,16 @@
         <v>144</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
@@ -15359,7 +15452,7 @@
       <c r="O146" s="1"/>
       <c r="P146" s="1"/>
       <c r="Q146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
@@ -15372,46 +15465,52 @@
       <c r="Z146" s="1"/>
       <c r="AA146" s="1"/>
       <c r="AB146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AC146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AD146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AE146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AF146" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AG146" s="1"/>
-      <c r="AH146" s="1"/>
+        <v>230</v>
+      </c>
+      <c r="AG146" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH146" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="AI146" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="AJ146" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="AJ146" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="AK146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AL146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AM146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AN146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AO146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AP146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AQ146" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AR146" s="1"/>
       <c r="AS146" s="1"/>
@@ -15450,16 +15549,16 @@
         <v>145</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -15473,7 +15572,7 @@
       <c r="O147" s="1"/>
       <c r="P147" s="1"/>
       <c r="Q147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
@@ -15486,46 +15585,52 @@
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
       <c r="AB147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AC147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AD147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AE147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AF147" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="AG147" s="1"/>
-      <c r="AH147" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="AG147" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH147" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="AI147" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="AJ147" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="AJ147" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="AK147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AL147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AM147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AN147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AO147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AP147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AQ147" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="AR147" s="1"/>
       <c r="AS147" s="1"/>
@@ -15564,16 +15669,16 @@
         <v>146</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
@@ -15587,7 +15692,7 @@
       <c r="O148" s="1"/>
       <c r="P148" s="1"/>
       <c r="Q148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
@@ -15600,50 +15705,52 @@
       <c r="Z148" s="1"/>
       <c r="AA148" s="1"/>
       <c r="AB148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AC148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AD148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AE148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AF148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AG148" s="1" t="s">
-        <v>197</v>
+        <v>270</v>
       </c>
       <c r="AH148" s="1" t="s">
-        <v>198</v>
+        <v>271</v>
       </c>
       <c r="AI148" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="AJ148" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="AJ148" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="AK148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AL148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AM148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AN148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AO148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AP148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AQ148" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AR148" s="1"/>
       <c r="AS148" s="1"/>
@@ -15682,16 +15789,16 @@
         <v>147</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
@@ -15705,7 +15812,7 @@
       <c r="O149" s="1"/>
       <c r="P149" s="1"/>
       <c r="Q149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="R149" s="1"/>
       <c r="S149" s="1"/>
@@ -15718,50 +15825,52 @@
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
       <c r="AB149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AC149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AD149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AE149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AF149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AG149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AH149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AI149" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="AJ149" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="AJ149" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="AK149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AL149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AM149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AN149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AO149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AP149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AQ149" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AR149" s="1"/>
       <c r="AS149" s="1"/>
@@ -15800,16 +15909,16 @@
         <v>148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
@@ -15823,7 +15932,7 @@
       <c r="O150" s="1"/>
       <c r="P150" s="1"/>
       <c r="Q150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="R150" s="1"/>
       <c r="S150" s="1"/>
@@ -15836,50 +15945,52 @@
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
       <c r="AB150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AC150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AD150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AE150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AF150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AG150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AH150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AI150" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="AJ150" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="AJ150" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="AK150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AL150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AM150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AN150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AO150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AP150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AQ150" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="AR150" s="1"/>
       <c r="AS150" s="1"/>
@@ -15918,16 +16029,16 @@
         <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -15941,7 +16052,7 @@
       <c r="O151" s="1"/>
       <c r="P151" s="1"/>
       <c r="Q151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
@@ -15953,55 +16064,55 @@
       <c r="Y151" s="1"/>
       <c r="Z151" s="1"/>
       <c r="AA151" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="AB151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AC151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AD151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AE151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AF151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AG151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AH151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AI151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AJ151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AK151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AL151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AM151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AN151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AO151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AP151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AQ151" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="AR151" s="1"/>
       <c r="AS151" s="1"/>
@@ -16040,16 +16151,16 @@
         <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
@@ -16063,7 +16174,7 @@
       <c r="O152" s="1"/>
       <c r="P152" s="1"/>
       <c r="Q152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="R152" s="1"/>
       <c r="S152" s="1"/>
@@ -16076,52 +16187,52 @@
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
       <c r="AB152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AC152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AD152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AE152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AF152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AG152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AH152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AI152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AJ152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AK152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AL152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AM152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AN152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AO152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AP152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AQ152" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="AR152" s="1"/>
       <c r="AS152" s="1"/>
@@ -16163,7 +16274,7 @@
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
@@ -16380,35 +16491,35 @@
         <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
       <c r="I155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="J155" s="1"/>
       <c r="K155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="M155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="O155" s="1"/>
       <c r="P155" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
@@ -16871,7 +16982,7 @@
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
@@ -16963,7 +17074,7 @@
       <c r="O160" s="1"/>
       <c r="P160" s="1"/>
       <c r="Q160" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
@@ -17028,7 +17139,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
@@ -17061,10 +17172,14 @@
       <c r="AC161" s="1"/>
       <c r="AD161" s="1"/>
       <c r="AE161" s="1"/>
-      <c r="AF161" s="1"/>
+      <c r="AF161" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="AG161" s="1"/>
       <c r="AH161" s="1"/>
-      <c r="AI161" s="1"/>
+      <c r="AI161" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AJ161" s="1"/>
       <c r="AK161" s="1" t="s">
         <v>164</v>
@@ -17109,16 +17224,32 @@
       <c r="BK161" s="1"/>
       <c r="BL161" s="1"/>
       <c r="BM161" s="1"/>
-      <c r="BN161" s="1"/>
-      <c r="BO161" s="1"/>
-      <c r="BP161" s="1"/>
-      <c r="BQ161" s="1"/>
-      <c r="BR161" s="1"/>
-      <c r="BS161" s="1"/>
-      <c r="BT161" s="1"/>
-      <c r="BU161" s="1"/>
+      <c r="BN161" s="1">
+        <v>166</v>
+      </c>
+      <c r="BO161" s="1">
+        <v>86</v>
+      </c>
+      <c r="BP161" s="1">
+        <v>87</v>
+      </c>
+      <c r="BQ161" s="1">
+        <v>88</v>
+      </c>
+      <c r="BR161" s="1">
+        <v>89</v>
+      </c>
+      <c r="BS161" s="1">
+        <v>90</v>
+      </c>
+      <c r="BT161" s="1">
+        <v>91</v>
+      </c>
+      <c r="BU161" s="1">
+        <v>94</v>
+      </c>
       <c r="BV161" s="1">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="162" spans="1:74" x14ac:dyDescent="0.25">
@@ -17126,16 +17257,16 @@
         <v>160</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -17149,7 +17280,7 @@
       <c r="O162" s="1"/>
       <c r="P162" s="1"/>
       <c r="Q162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="R162" s="1"/>
       <c r="S162" s="1"/>
@@ -17162,52 +17293,52 @@
       <c r="Z162" s="1"/>
       <c r="AA162" s="1"/>
       <c r="AB162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AC162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AD162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AE162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AF162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AG162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AH162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AI162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AJ162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AK162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AL162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AM162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AN162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AO162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AP162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AQ162" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AR162" s="1"/>
       <c r="AS162" s="1"/>
@@ -17246,69 +17377,69 @@
         <v>161</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E163" s="1"/>
       <c r="F163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="M163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="O163" s="1"/>
       <c r="P163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
       <c r="S163" s="1"/>
       <c r="T163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="U163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="V163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="W163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="X163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="Y163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="Z163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
@@ -17316,37 +17447,37 @@
       <c r="AD163" s="1"/>
       <c r="AE163" s="1"/>
       <c r="AF163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AG163" s="1"/>
       <c r="AH163" s="1"/>
       <c r="AI163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AJ163" s="1"/>
       <c r="AK163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AL163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AM163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AN163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AO163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AP163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AQ163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AR163" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AS163" s="1"/>
       <c r="AT163" s="1"/>
@@ -17384,22 +17515,22 @@
         <v>162</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
@@ -17412,25 +17543,25 @@
       <c r="R164" s="1"/>
       <c r="S164" s="1"/>
       <c r="T164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="U164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="V164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="W164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="X164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="Y164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="Z164" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AA164" s="1"/>
       <c r="AB164" s="1"/>
@@ -17438,34 +17569,34 @@
       <c r="AD164" s="1"/>
       <c r="AE164" s="1"/>
       <c r="AF164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AG164" s="1"/>
       <c r="AH164" s="1"/>
       <c r="AI164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AJ164" s="1"/>
       <c r="AK164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AL164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AM164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AN164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AO164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AP164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AQ164" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AR164" s="1"/>
       <c r="AS164" s="1"/>
@@ -17506,22 +17637,22 @@
         <v>163</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
@@ -17534,25 +17665,25 @@
       <c r="R165" s="1"/>
       <c r="S165" s="1"/>
       <c r="T165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="U165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="V165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="W165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="X165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="Y165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="Z165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AA165" s="1"/>
       <c r="AB165" s="1"/>
@@ -17560,34 +17691,34 @@
       <c r="AD165" s="1"/>
       <c r="AE165" s="1"/>
       <c r="AF165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AG165" s="1"/>
       <c r="AH165" s="1"/>
       <c r="AI165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AJ165" s="1"/>
       <c r="AK165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AL165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AM165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AN165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AO165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AP165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AQ165" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="AR165" s="1"/>
       <c r="AS165" s="1"/>
@@ -17627,7 +17758,7 @@
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -17707,7 +17838,7 @@
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -17786,16 +17917,16 @@
         <v>166</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -17809,7 +17940,7 @@
       <c r="O168" s="1"/>
       <c r="P168" s="1"/>
       <c r="Q168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="R168" s="1"/>
       <c r="S168" s="1"/>
@@ -17822,52 +17953,52 @@
       <c r="Z168" s="1"/>
       <c r="AA168" s="1"/>
       <c r="AB168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AC168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AD168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AE168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AF168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AG168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AH168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AI168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AJ168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AK168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AL168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AM168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AN168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AO168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AP168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AQ168" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AR168" s="1"/>
       <c r="AS168" s="1"/>
@@ -17906,22 +18037,22 @@
         <v>167</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
@@ -17934,25 +18065,25 @@
       <c r="R169" s="1"/>
       <c r="S169" s="1"/>
       <c r="T169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="U169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="V169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="W169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="X169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="Y169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="Z169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
@@ -17960,34 +18091,34 @@
       <c r="AD169" s="1"/>
       <c r="AE169" s="1"/>
       <c r="AF169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AG169" s="1"/>
       <c r="AH169" s="1"/>
       <c r="AI169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AJ169" s="1"/>
       <c r="AK169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AL169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AM169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AN169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AO169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AP169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AQ169" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AR169" s="1"/>
       <c r="AS169" s="1"/>
@@ -18282,22 +18413,22 @@
         <v>170</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
@@ -18310,25 +18441,25 @@
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
       <c r="T172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="U172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="V172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="W172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="X172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="Y172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="Z172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
@@ -18336,34 +18467,34 @@
       <c r="AD172" s="1"/>
       <c r="AE172" s="1"/>
       <c r="AF172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AG172" s="1"/>
       <c r="AH172" s="1"/>
       <c r="AI172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AJ172" s="1"/>
       <c r="AK172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AL172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AM172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AN172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AO172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AP172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AQ172" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AR172" s="1"/>
       <c r="AS172" s="1"/>
@@ -18402,22 +18533,22 @@
         <v>171</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
@@ -18430,25 +18561,25 @@
       <c r="R173" s="1"/>
       <c r="S173" s="1"/>
       <c r="T173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="U173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="V173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="W173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="X173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="Y173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="Z173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
@@ -18456,34 +18587,34 @@
       <c r="AD173" s="1"/>
       <c r="AE173" s="1"/>
       <c r="AF173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AG173" s="1"/>
       <c r="AH173" s="1"/>
       <c r="AI173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AJ173" s="1"/>
       <c r="AK173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AL173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AM173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AN173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AO173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AP173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AQ173" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AR173" s="1"/>
       <c r="AS173" s="1"/>
@@ -18525,7 +18656,7 @@
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
@@ -18740,22 +18871,22 @@
         <v>174</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
@@ -18768,25 +18899,25 @@
       <c r="R176" s="1"/>
       <c r="S176" s="1"/>
       <c r="T176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="U176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="V176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="W176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="X176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="Y176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="Z176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
@@ -18794,34 +18925,34 @@
       <c r="AD176" s="1"/>
       <c r="AE176" s="1"/>
       <c r="AF176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AG176" s="1"/>
       <c r="AH176" s="1"/>
       <c r="AI176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AJ176" s="1"/>
       <c r="AK176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AL176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AM176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AN176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AO176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AP176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AQ176" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AR176" s="1"/>
       <c r="AS176" s="1"/>

</xml_diff>